<commit_message>
Re-run scripts to ensure final data files only contain -99 as missing symbol
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMSS_2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED0CE9C-3714-438F-A678-FBDA6001926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D9F3DF-B127-4C2F-B7C9-41BF666590E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="730" activeTab="8" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="730" activeTab="2" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
   </bookViews>
   <sheets>
     <sheet name="1_G4_PV" sheetId="14" r:id="rId1"/>
@@ -11257,7 +11257,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11267,12 +11267,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11301,7 +11295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -11340,19 +11334,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -14295,7 +14286,7 @@
       <c r="B37" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="17" t="s">
         <v>3686</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -14318,7 +14309,7 @@
       <c r="B38" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="17" t="s">
         <v>3687</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -14341,7 +14332,7 @@
       <c r="B39" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="17" t="s">
         <v>3688</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -14364,7 +14355,7 @@
       <c r="B40" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="17" t="s">
         <v>3689</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -14387,7 +14378,7 @@
       <c r="B41" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>3690</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -14410,7 +14401,7 @@
       <c r="B42" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="17" t="s">
         <v>3691</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -14433,7 +14424,7 @@
       <c r="B43" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="17" t="s">
         <v>3692</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -14456,7 +14447,7 @@
       <c r="B44" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="17" t="s">
         <v>3693</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -14479,7 +14470,7 @@
       <c r="B45" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="17" t="s">
         <v>3694</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -14502,7 +14493,7 @@
       <c r="B46" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="17" t="s">
         <v>3695</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -14525,7 +14516,7 @@
       <c r="B47" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="17" t="s">
         <v>3696</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -15228,7 +15219,7 @@
       <c r="B78" s="2" t="s">
         <v>2041</v>
       </c>
-      <c r="C78" s="18" t="s">
+      <c r="C78" s="17" t="s">
         <v>3697</v>
       </c>
       <c r="D78" s="2" t="s">
@@ -15314,7 +15305,7 @@
       <c r="B82" s="2" t="s">
         <v>2041</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C82" s="17" t="s">
         <v>3698</v>
       </c>
       <c r="D82" s="2" t="s">
@@ -15800,7 +15791,7 @@
       <c r="B16" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>3635</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -15823,7 +15814,7 @@
       <c r="B17" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>3636</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -15846,7 +15837,7 @@
       <c r="B18" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>3637</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -15869,7 +15860,7 @@
       <c r="B19" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>3638</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -15892,7 +15883,7 @@
       <c r="B20" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>3639</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -15915,7 +15906,7 @@
       <c r="B21" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>3640</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -15938,7 +15929,7 @@
       <c r="B22" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>3641</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -15961,7 +15952,7 @@
       <c r="B23" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>3642</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -15984,7 +15975,7 @@
       <c r="B24" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>3643</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -16007,7 +15998,7 @@
       <c r="B25" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>3644</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -16030,7 +16021,7 @@
       <c r="B26" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>3645</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -16053,7 +16044,7 @@
       <c r="B27" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>3646</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -17795,7 +17786,7 @@
       <c r="D103" s="2" t="s">
         <v>859</v>
       </c>
-      <c r="E103" s="15" t="s">
+      <c r="E103" s="14" t="s">
         <v>1507</v>
       </c>
       <c r="F103" s="3">
@@ -19517,7 +19508,7 @@
       <c r="D178" s="2" t="s">
         <v>934</v>
       </c>
-      <c r="E178" s="15" t="s">
+      <c r="E178" s="14" t="s">
         <v>1507</v>
       </c>
       <c r="F178" s="3">
@@ -20138,7 +20129,7 @@
       <c r="D205" s="2" t="s">
         <v>961</v>
       </c>
-      <c r="E205" s="15" t="s">
+      <c r="E205" s="14" t="s">
         <v>3619</v>
       </c>
       <c r="F205" s="3">
@@ -20189,7 +20180,7 @@
       <c r="B208" s="2" t="s">
         <v>1626</v>
       </c>
-      <c r="C208" s="14" t="s">
+      <c r="C208" s="13" t="s">
         <v>3658</v>
       </c>
       <c r="D208" s="2" t="s">
@@ -20209,7 +20200,7 @@
       <c r="B209" s="2" t="s">
         <v>1626</v>
       </c>
-      <c r="C209" s="14" t="s">
+      <c r="C209" s="13" t="s">
         <v>3659</v>
       </c>
       <c r="D209" s="2" t="s">
@@ -20387,7 +20378,7 @@
       <c r="D217" s="2" t="s">
         <v>973</v>
       </c>
-      <c r="E217" s="15" t="s">
+      <c r="E217" s="14" t="s">
         <v>1505</v>
       </c>
       <c r="F217" s="3">
@@ -20577,9 +20568,9 @@
   </sheetPr>
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21268,7 +21259,7 @@
       <c r="B30" s="2" t="s">
         <v>1684</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>3660</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -21314,7 +21305,7 @@
       <c r="B32" s="2" t="s">
         <v>1684</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>3661</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -21337,7 +21328,7 @@
       <c r="B33" s="2" t="s">
         <v>1684</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>3662</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -21935,7 +21926,7 @@
       <c r="B59" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="13" t="s">
         <v>3663</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -22073,7 +22064,7 @@
       <c r="B65" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="13" t="s">
         <v>3664</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -23143,7 +23134,7 @@
         <v>1653</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>1652</v>
+        <v>3724</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>1089</v>
@@ -23403,7 +23394,7 @@
       <c r="B127" s="2" t="s">
         <v>2014</v>
       </c>
-      <c r="C127" s="14" t="s">
+      <c r="C127" s="13" t="s">
         <v>3634</v>
       </c>
       <c r="D127" s="2" t="s">
@@ -23704,7 +23695,7 @@
       <c r="B141" s="5" t="s">
         <v>2021</v>
       </c>
-      <c r="C141" s="14" t="s">
+      <c r="C141" s="13" t="s">
         <v>3632</v>
       </c>
       <c r="D141" s="5" t="s">
@@ -23724,7 +23715,7 @@
       <c r="B142" s="5" t="s">
         <v>2021</v>
       </c>
-      <c r="C142" s="14" t="s">
+      <c r="C142" s="13" t="s">
         <v>3633</v>
       </c>
       <c r="D142" s="5" t="s">
@@ -24310,11 +24301,11 @@
       <c r="D21" s="2" t="s">
         <v>1142</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="3" t="s">
         <v>1635</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>3384</v>
       </c>
     </row>
@@ -24791,7 +24782,7 @@
       <c r="D42" s="2" t="s">
         <v>1160</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="14" t="s">
         <v>1461</v>
       </c>
       <c r="F42" s="3">
@@ -24814,7 +24805,7 @@
       <c r="D43" s="2" t="s">
         <v>1161</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="14" t="s">
         <v>1461</v>
       </c>
       <c r="F43" s="3">
@@ -25205,7 +25196,7 @@
       <c r="D60" s="2" t="s">
         <v>1178</v>
       </c>
-      <c r="E60" s="15" t="s">
+      <c r="E60" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F60" s="3" t="s">
@@ -25228,7 +25219,7 @@
       <c r="D61" s="2" t="s">
         <v>1179</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F61" s="3" t="s">
@@ -25251,7 +25242,7 @@
       <c r="D62" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -25274,7 +25265,7 @@
       <c r="D63" s="2" t="s">
         <v>1181</v>
       </c>
-      <c r="E63" s="15" t="s">
+      <c r="E63" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -25297,7 +25288,7 @@
       <c r="D64" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E64" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -25320,7 +25311,7 @@
       <c r="D65" s="2" t="s">
         <v>1181</v>
       </c>
-      <c r="E65" s="15" t="s">
+      <c r="E65" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F65" s="3" t="s">
@@ -25343,7 +25334,7 @@
       <c r="D66" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F66" s="3" t="s">
@@ -25366,7 +25357,7 @@
       <c r="D67" s="2" t="s">
         <v>1181</v>
       </c>
-      <c r="E67" s="15" t="s">
+      <c r="E67" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F67" s="3" t="s">
@@ -25389,7 +25380,7 @@
       <c r="D68" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="E68" s="15" t="s">
+      <c r="E68" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F68" s="3" t="s">
@@ -25412,7 +25403,7 @@
       <c r="D69" s="2" t="s">
         <v>1181</v>
       </c>
-      <c r="E69" s="15" t="s">
+      <c r="E69" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -25435,7 +25426,7 @@
       <c r="D70" s="2" t="s">
         <v>1182</v>
       </c>
-      <c r="E70" s="15" t="s">
+      <c r="E70" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F70" s="3" t="s">
@@ -25458,7 +25449,7 @@
       <c r="D71" s="2" t="s">
         <v>1183</v>
       </c>
-      <c r="E71" s="15" t="s">
+      <c r="E71" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F71" s="3" t="s">
@@ -25481,7 +25472,7 @@
       <c r="D72" s="2" t="s">
         <v>1184</v>
       </c>
-      <c r="E72" s="15" t="s">
+      <c r="E72" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F72" s="3" t="s">
@@ -25504,7 +25495,7 @@
       <c r="D73" s="2" t="s">
         <v>1185</v>
       </c>
-      <c r="E73" s="15" t="s">
+      <c r="E73" s="14" t="s">
         <v>3665</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -26006,7 +25997,7 @@
       <c r="D96" s="2" t="s">
         <v>1208</v>
       </c>
-      <c r="E96" s="15" t="s">
+      <c r="E96" s="14" t="s">
         <v>3666</v>
       </c>
       <c r="F96" s="3">
@@ -26884,7 +26875,7 @@
       <c r="B36" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>3647</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -26907,7 +26898,7 @@
       <c r="B37" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>3648</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -26930,7 +26921,7 @@
       <c r="B38" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>3649</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -26953,7 +26944,7 @@
       <c r="B39" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>3650</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -26976,7 +26967,7 @@
       <c r="B40" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>3651</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -26999,7 +26990,7 @@
       <c r="B41" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>3652</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -27022,7 +27013,7 @@
       <c r="B42" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>3653</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -27045,7 +27036,7 @@
       <c r="B43" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>3654</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -27068,7 +27059,7 @@
       <c r="B44" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>3655</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -27091,7 +27082,7 @@
       <c r="B45" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>3656</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -27114,7 +27105,7 @@
       <c r="B46" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>3657</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -28432,12 +28423,12 @@
       <c r="G20" s="2" t="s">
         <v>1781</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="15" t="s">
         <v>3667</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -30396,7 +30387,7 @@
       <c r="B15" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>3672</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -30419,7 +30410,7 @@
       <c r="B16" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>3673</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -30442,7 +30433,7 @@
       <c r="B17" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>3674</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -30465,7 +30456,7 @@
       <c r="B18" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>3675</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -30488,7 +30479,7 @@
       <c r="B19" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>3676</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -30511,7 +30502,7 @@
       <c r="B20" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>3677</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -30534,7 +30525,7 @@
       <c r="B21" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>3678</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -30557,7 +30548,7 @@
       <c r="B22" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>3679</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -30580,7 +30571,7 @@
       <c r="B23" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>3680</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -30603,7 +30594,7 @@
       <c r="B24" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="17" t="s">
         <v>3681</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -30626,7 +30617,7 @@
       <c r="B25" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="17" t="s">
         <v>3682</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -30649,7 +30640,7 @@
       <c r="B26" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>3683</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -32112,7 +32103,7 @@
       <c r="B90" s="2" t="s">
         <v>1464</v>
       </c>
-      <c r="C90" s="18" t="s">
+      <c r="C90" s="17" t="s">
         <v>3668</v>
       </c>
       <c r="D90" s="2" t="s">
@@ -32135,7 +32126,7 @@
       <c r="B91" s="2" t="s">
         <v>1464</v>
       </c>
-      <c r="C91" s="18" t="s">
+      <c r="C91" s="17" t="s">
         <v>3669</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -32342,7 +32333,7 @@
       <c r="B100" s="2" t="s">
         <v>1464</v>
       </c>
-      <c r="C100" s="18" t="s">
+      <c r="C100" s="17" t="s">
         <v>3670</v>
       </c>
       <c r="D100" s="2" t="s">
@@ -33135,7 +33126,7 @@
       <c r="B135" s="2" t="s">
         <v>3169</v>
       </c>
-      <c r="C135" s="18" t="s">
+      <c r="C135" s="17" t="s">
         <v>3684</v>
       </c>
       <c r="D135" s="2" t="s">
@@ -33215,7 +33206,7 @@
       <c r="B139" s="2" t="s">
         <v>3173</v>
       </c>
-      <c r="C139" s="18" t="s">
+      <c r="C139" s="17" t="s">
         <v>3685</v>
       </c>
       <c r="D139" s="2" t="s">
@@ -33760,7 +33751,7 @@
       <c r="B15" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>3699</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -33783,7 +33774,7 @@
       <c r="B16" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>3700</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -33806,7 +33797,7 @@
       <c r="B17" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>3701</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -33829,7 +33820,7 @@
       <c r="B18" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>3702</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -33852,7 +33843,7 @@
       <c r="B19" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>3703</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -33875,7 +33866,7 @@
       <c r="B20" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>3704</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -33898,7 +33889,7 @@
       <c r="B21" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>3705</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -33921,7 +33912,7 @@
       <c r="B22" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>3706</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -33944,7 +33935,7 @@
       <c r="B23" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>3707</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -33967,7 +33958,7 @@
       <c r="B24" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="17" t="s">
         <v>3708</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -33990,7 +33981,7 @@
       <c r="B25" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="17" t="s">
         <v>3709</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -34013,7 +34004,7 @@
       <c r="B26" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>3710</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -34906,7 +34897,7 @@
       <c r="B65" s="2" t="s">
         <v>3572</v>
       </c>
-      <c r="C65" s="18" t="s">
+      <c r="C65" s="17" t="s">
         <v>3671</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -36713,7 +36704,7 @@
       <c r="B144" s="2" t="s">
         <v>3169</v>
       </c>
-      <c r="C144" s="18" t="s">
+      <c r="C144" s="17" t="s">
         <v>3711</v>
       </c>
       <c r="D144" s="2" t="s">
@@ -36818,7 +36809,7 @@
       <c r="B149" s="2" t="s">
         <v>3174</v>
       </c>
-      <c r="C149" s="18" t="s">
+      <c r="C149" s="17" t="s">
         <v>3712</v>
       </c>
       <c r="D149" s="2" t="s">
@@ -37047,7 +37038,7 @@
   </sheetPr>
   <dimension ref="A1:G351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A283" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F298" sqref="F298"/>
     </sheetView>
@@ -38726,7 +38717,7 @@
       <c r="B73" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="17" t="s">
         <v>3663</v>
       </c>
       <c r="D73" s="2" t="s">
@@ -38864,7 +38855,7 @@
       <c r="B79" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="17" t="s">
         <v>3664</v>
       </c>
       <c r="D79" s="2" t="s">
@@ -39600,7 +39591,7 @@
       <c r="B111" s="2" t="s">
         <v>1719</v>
       </c>
-      <c r="C111" s="18" t="s">
+      <c r="C111" s="17" t="s">
         <v>3713</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -39623,7 +39614,7 @@
       <c r="B112" s="2" t="s">
         <v>1719</v>
       </c>
-      <c r="C112" s="18" t="s">
+      <c r="C112" s="17" t="s">
         <v>3714</v>
       </c>
       <c r="D112" s="2" t="s">
@@ -40589,7 +40580,7 @@
       <c r="B154" s="2" t="s">
         <v>3234</v>
       </c>
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="17" t="s">
         <v>3715</v>
       </c>
       <c r="D154" s="2" t="s">
@@ -40612,7 +40603,7 @@
       <c r="B155" s="2" t="s">
         <v>3234</v>
       </c>
-      <c r="C155" s="18" t="s">
+      <c r="C155" s="17" t="s">
         <v>3716</v>
       </c>
       <c r="D155" s="2" t="s">
@@ -40681,7 +40672,7 @@
       <c r="B158" s="2" t="s">
         <v>3247</v>
       </c>
-      <c r="C158" s="18" t="s">
+      <c r="C158" s="17" t="s">
         <v>3717</v>
       </c>
       <c r="D158" s="2" t="s">
@@ -41187,7 +41178,7 @@
       <c r="B180" s="2" t="s">
         <v>3251</v>
       </c>
-      <c r="C180" s="18" t="s">
+      <c r="C180" s="17" t="s">
         <v>3718</v>
       </c>
       <c r="D180" s="2" t="s">
@@ -41210,7 +41201,7 @@
       <c r="B181" s="2" t="s">
         <v>3251</v>
       </c>
-      <c r="C181" s="18" t="s">
+      <c r="C181" s="17" t="s">
         <v>3719</v>
       </c>
       <c r="D181" s="2" t="s">
@@ -41785,7 +41776,7 @@
       <c r="B206" s="2" t="s">
         <v>3280</v>
       </c>
-      <c r="C206" s="18" t="s">
+      <c r="C206" s="17" t="s">
         <v>3720</v>
       </c>
       <c r="D206" s="2" t="s">
@@ -41808,7 +41799,7 @@
       <c r="B207" s="2" t="s">
         <v>3280</v>
       </c>
-      <c r="C207" s="18" t="s">
+      <c r="C207" s="17" t="s">
         <v>3721</v>
       </c>
       <c r="D207" s="2" t="s">
@@ -42383,7 +42374,7 @@
       <c r="B232" s="2" t="s">
         <v>3310</v>
       </c>
-      <c r="C232" s="18" t="s">
+      <c r="C232" s="17" t="s">
         <v>3722</v>
       </c>
       <c r="D232" s="2" t="s">
@@ -42406,7 +42397,7 @@
       <c r="B233" s="2" t="s">
         <v>3310</v>
       </c>
-      <c r="C233" s="18" t="s">
+      <c r="C233" s="17" t="s">
         <v>3723</v>
       </c>
       <c r="D233" s="2" t="s">
@@ -43678,7 +43669,7 @@
       <c r="B289" s="2" t="s">
         <v>1653</v>
       </c>
-      <c r="C289" s="18" t="s">
+      <c r="C289" s="17" t="s">
         <v>3724</v>
       </c>
       <c r="D289" s="2" t="s">
@@ -43751,7 +43742,7 @@
       <c r="F292" s="3">
         <v>999999</v>
       </c>
-      <c r="G292" s="17" t="s">
+      <c r="G292" s="16" t="s">
         <v>3384</v>
       </c>
     </row>
@@ -43768,7 +43759,7 @@
       <c r="F293" s="3">
         <v>999999</v>
       </c>
-      <c r="G293" s="17" t="s">
+      <c r="G293" s="16" t="s">
         <v>3384</v>
       </c>
     </row>
@@ -43785,7 +43776,7 @@
       <c r="F294" s="3">
         <v>999999</v>
       </c>
-      <c r="G294" s="17" t="s">
+      <c r="G294" s="16" t="s">
         <v>3384</v>
       </c>
     </row>
@@ -43802,7 +43793,7 @@
       <c r="F295" s="3">
         <v>999999</v>
       </c>
-      <c r="G295" s="17" t="s">
+      <c r="G295" s="16" t="s">
         <v>3384</v>
       </c>
     </row>
@@ -43819,7 +43810,7 @@
       <c r="F296" s="3">
         <v>999999</v>
       </c>
-      <c r="G296" s="17" t="s">
+      <c r="G296" s="16" t="s">
         <v>3384</v>
       </c>
     </row>
@@ -43836,7 +43827,7 @@
       <c r="F297" s="3">
         <v>999999</v>
       </c>
-      <c r="G297" s="17" t="s">
+      <c r="G297" s="16" t="s">
         <v>3384</v>
       </c>
     </row>
@@ -44020,10 +44011,10 @@
       <c r="A306" s="2" t="s">
         <v>2626</v>
       </c>
-      <c r="B306" s="17" t="s">
+      <c r="B306" s="16" t="s">
         <v>2013</v>
       </c>
-      <c r="C306" s="18" t="s">
+      <c r="C306" s="17" t="s">
         <v>1790</v>
       </c>
       <c r="D306" s="2" t="s">
@@ -44041,10 +44032,10 @@
       <c r="A307" s="2" t="s">
         <v>2627</v>
       </c>
-      <c r="B307" s="17" t="s">
+      <c r="B307" s="16" t="s">
         <v>2013</v>
       </c>
-      <c r="C307" s="18" t="s">
+      <c r="C307" s="17" t="s">
         <v>1791</v>
       </c>
       <c r="D307" s="2" t="s">

</xml_diff>